<commit_message>
agregar product data, lista de productos y seleccionar producto
</commit_message>
<xml_diff>
--- a/WishCasosPrueba.xlsx
+++ b/WishCasosPrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kvvq373\repo\WishFinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D959085-A082-4CC8-882E-4AAF974DAFE2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22301C40-2793-4DDD-AFD8-A48D1D670619}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WishLogin" sheetId="3" r:id="rId1"/>
@@ -585,7 +585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B298572C-4BA0-4B18-86A0-0B768DFB429D}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941B164B-57B5-47A8-B908-90A18B3F7B93}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.33203125" defaultRowHeight="15.05"/>

</xml_diff>